<commit_message>
updated code with changes
</commit_message>
<xml_diff>
--- a/device_input_data.xlsx
+++ b/device_input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandanandan/PycharmProjects/tr_automation/telnet-cisco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61575C90-78E7-9E48-9E34-5496DEB52CB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A0F259-4F42-3D44-8E42-B89B269DDA8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="460" windowWidth="32560" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>IP</t>
   </si>
@@ -29,12 +29,6 @@
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>Ping</t>
-  </si>
-  <si>
-    <t>Change</t>
   </si>
   <si>
     <t>10.189.5.155</t>
@@ -388,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -399,7 +393,7 @@
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,30 +403,20 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>